<commit_message>
Add new feature file
</commit_message>
<xml_diff>
--- a/Data/HotelDataDetails.xlsx
+++ b/Data/HotelDataDetails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shanm\eclipse-workspace\AdcatinHotelCucumber\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inahosolutions0-my.sharepoint.com/personal/k-shanmathi_inahosolutions_com/Documents/Shanmathi/AutomationProject/Cucumber_AdactinHotel/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9A8C27-3CA6-4C8E-80D9-0E42FE59154D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{BA9A8C27-3CA6-4C8E-80D9-0E42FE59154D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E42D61F-3AD5-48F8-AAD2-0D1304915ED3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{884E7A26-A25A-4958-85BC-927675D72C8E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{884E7A26-A25A-4958-85BC-927675D72C8E}"/>
   </bookViews>
   <sheets>
     <sheet name="BookingDetails" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>AM29JB</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -139,6 +136,10 @@
   </si>
   <si>
     <t>Shanmathi22</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>E9Z51L</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -224,7 +225,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -251,12 +252,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -594,29 +589,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA236FED-F4DC-48BB-B911-7187FF9B3048}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="2" width="12.796875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.09765625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.296875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.3984375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.59765625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.3984375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.296875" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" width="12.75" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.25" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.25" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="14.5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.09765625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.3984375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.375" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="16" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="15.5" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="10.19921875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="10.09765625" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="12.09765625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="29.8984375" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="10.25" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.125" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.125" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="29.875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -627,74 +622,74 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="K1" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="G2" s="3">
         <v>45351</v>
@@ -703,28 +698,28 @@
         <v>45352</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="Q2" s="2">
         <v>2027</v>
@@ -732,8 +727,6 @@
       <c r="R2" s="1">
         <v>356</v>
       </c>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>